<commit_message>
Bug and task metrics updated
</commit_message>
<xml_diff>
--- a/metrics/tm.xlsx
+++ b/metrics/tm.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amanda\Desktop\SE\SE\is203-2017_G1T3\metrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel Tay\Desktop\SMU\SEM 2.1\SE\SE Project\is203-2017_G1T3\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" xr2:uid="{DFC5EB72-3D95-4787-93D0-40B9C90E77C7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945" xr2:uid="{DFC5EB72-3D95-4787-93D0-40B9C90E77C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Task Metrics" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Iteration</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t xml:space="preserve">As some of these tasks were still undone from iteration 2, we had moved these spillover tasks to the next iteration. We also rearranged some of the functionalities that we wanted to carry out in iteration 3 to iteration 5 instead. </t>
+  </si>
+  <si>
+    <t>Our estimates are fairly accurate, the team are roughly on track. There are a few unplanned tasks that were created along the way, hence spilling over some tasks to the next iteration. Buffer days are sufficient</t>
   </si>
 </sst>
 </file>
@@ -246,9 +249,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>78328</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>134697</xdr:rowOff>
+      <xdr:colOff>78329</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>322982</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -584,20 +587,20 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="E7" sqref="E7:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.26953125" customWidth="1"/>
-    <col min="6" max="6" width="31" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
@@ -607,7 +610,7 @@
       <c r="E1" s="10"/>
       <c r="F1" s="11"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -627,7 +630,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -648,7 +651,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -669,22 +672,28 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" s="4">
         <v>43018</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6" t="e">
+      <c r="C5" s="5">
+        <v>24</v>
+      </c>
+      <c r="D5" s="5">
+        <v>22</v>
+      </c>
+      <c r="E5" s="6">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F5" s="8"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -699,7 +708,7 @@
       </c>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -709,12 +718,12 @@
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="6" t="e">
-        <f t="shared" ref="E7" si="1">D7/C7</f>
+        <f t="shared" ref="E7:E9" si="1">D7/C7</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -723,10 +732,13 @@
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="6"/>
+      <c r="E8" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -735,7 +747,10 @@
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
-      <c r="E9" s="6"/>
+      <c r="E9" s="6" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="F9" s="8"/>
     </row>
   </sheetData>

</xml_diff>